<commit_message>
colocando o nome do orçamentista no logging
</commit_message>
<xml_diff>
--- a/PlanDist.xlsx
+++ b/PlanDist.xlsx
@@ -9938,7 +9938,7 @@
       <c r="B3" s="111" t="n"/>
       <c r="C3" s="112" t="inlineStr">
         <is>
-          <t>Luiz Henrique</t>
+          <t>Felipe Almeida</t>
         </is>
       </c>
       <c r="D3" s="113" t="n"/>
@@ -9968,7 +9968,7 @@
       <c r="B4" s="111" t="n"/>
       <c r="C4" s="112" t="inlineStr">
         <is>
-          <t>Luan Araujo</t>
+          <t>Wellisson Chaves</t>
         </is>
       </c>
       <c r="D4" s="113" t="n"/>
@@ -9994,7 +9994,7 @@
       <c r="B5" s="111" t="n"/>
       <c r="C5" s="76" t="inlineStr">
         <is>
-          <t>1017</t>
+          <t>1020</t>
         </is>
       </c>
       <c r="E5" s="21" t="n"/>
@@ -10238,7 +10238,7 @@
       </c>
       <c r="D11" s="33" t="inlineStr">
         <is>
-          <t>010 CAIXA VAV TVJEASY 1000x307  TROX</t>
+          <t>010 TOMADA DE AR VDF F711 AWG 597x597  TROX</t>
         </is>
       </c>
       <c r="E11" s="33" t="inlineStr">
@@ -10252,20 +10252,20 @@
       </c>
       <c r="G11" s="33" t="inlineStr">
         <is>
-          <t>TVJEASY/1000x307</t>
+          <t>VDF-F711/597x597/G/AG/F/AN0</t>
         </is>
       </c>
       <c r="H11" s="33" t="n">
-        <v>90261029</v>
+        <v>76169900</v>
       </c>
       <c r="I11" s="34" t="n">
-        <v>1997.3</v>
+        <v>488.82</v>
       </c>
       <c r="J11" s="35" t="n">
         <v>0</v>
       </c>
       <c r="K11" s="35" t="n">
-        <v>0</v>
+        <v>0.0325</v>
       </c>
       <c r="L11" s="36">
         <f>IF($H$4="-",0,IF($H$4="VAREJO",AW11,IF($H$4="ATACADO",AX11,0)))</f>
@@ -10355,7 +10355,7 @@
       </c>
       <c r="D12" s="33" t="inlineStr">
         <is>
-          <t>010 TERMOSTATO GS7.02.S GLOBUS TROX</t>
+          <t>010 TOMADA DE AR VDF F711 AWG 497x497  TROX</t>
         </is>
       </c>
       <c r="E12" s="33" t="inlineStr">
@@ -10369,22 +10369,20 @@
       </c>
       <c r="G12" s="33" t="inlineStr">
         <is>
-          <t>TERMOSTATO GS7.02.S GLOBUS</t>
-        </is>
-      </c>
-      <c r="H12" s="33" t="inlineStr">
-        <is>
-          <t>COLOCAR NCM</t>
-        </is>
+          <t>VDF-F711/497x497/G/AG/F/AN0</t>
+        </is>
+      </c>
+      <c r="H12" s="33" t="n">
+        <v>76169900</v>
       </c>
       <c r="I12" s="46" t="n">
-        <v>305.08</v>
+        <v>405.67</v>
       </c>
       <c r="J12" s="35" t="n">
         <v>0</v>
       </c>
       <c r="K12" s="35" t="n">
-        <v>0.0975</v>
+        <v>0.0325</v>
       </c>
       <c r="L12" s="36">
         <f>IF($H$4="-",0,IF($H$4="VAREJO",AW12,IF($H$4="ATACADO",AX12,0)))</f>
@@ -10465,7 +10463,7 @@
         <v>3</v>
       </c>
       <c r="B13" s="33" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C13" s="33" t="inlineStr">
         <is>
@@ -10474,7 +10472,7 @@
       </c>
       <c r="D13" s="33" t="inlineStr">
         <is>
-          <t>010 DAMPER JN-A M 1200x300 00 000 TROX</t>
+          <t>010 DAMPER JN-A 0 700x250 00 000 TROX</t>
         </is>
       </c>
       <c r="E13" s="33" t="inlineStr">
@@ -10488,14 +10486,14 @@
       </c>
       <c r="G13" s="33" t="inlineStr">
         <is>
-          <t>JN-A-M-D-N0/1200x300/N/00/000</t>
+          <t>JN-A-0-D-N0/700x250/N/00/000</t>
         </is>
       </c>
       <c r="H13" s="33" t="n">
         <v>90261029</v>
       </c>
       <c r="I13" s="46" t="n">
-        <v>563.35</v>
+        <v>314.28</v>
       </c>
       <c r="J13" s="35" t="n">
         <v>0</v>
@@ -10582,7 +10580,7 @@
         <v>4</v>
       </c>
       <c r="B14" s="33" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C14" s="33" t="inlineStr">
         <is>
@@ -10591,7 +10589,7 @@
       </c>
       <c r="D14" s="33" t="inlineStr">
         <is>
-          <t>010 DIFUSOR VD V 600 AN0 TROX</t>
+          <t>010 DAMPER JN-A 0 400x250 00 000 TROX</t>
         </is>
       </c>
       <c r="E14" s="33" t="inlineStr">
@@ -10605,20 +10603,20 @@
       </c>
       <c r="G14" s="33" t="inlineStr">
         <is>
-          <t>VD-V-0-0-0/600/00/AN0/0/0</t>
+          <t>JN-A-0-D-N0/400x250/N/00/000</t>
         </is>
       </c>
       <c r="H14" s="33" t="n">
-        <v>76169900</v>
+        <v>90261029</v>
       </c>
       <c r="I14" s="46" t="n">
-        <v>825.33</v>
+        <v>247.23</v>
       </c>
       <c r="J14" s="35" t="n">
         <v>0</v>
       </c>
       <c r="K14" s="35" t="n">
-        <v>0.0325</v>
+        <v>0</v>
       </c>
       <c r="L14" s="36">
         <f>IF($H$4="-",0,IF($H$4="VAREJO",AW14,IF($H$4="ATACADO",AX14,0)))</f>
@@ -10708,12 +10706,12 @@
       </c>
       <c r="D15" s="33" t="inlineStr">
         <is>
-          <t>010 DIFUSOR ADLQ T5MM AG 0 AN0 TROX</t>
+          <t>010 DAMPER JN-A 0 350x250 00 000 TROX</t>
         </is>
       </c>
       <c r="E15" s="33" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>C</t>
         </is>
       </c>
       <c r="F15" s="71">
@@ -10722,20 +10720,20 @@
       </c>
       <c r="G15" s="33" t="inlineStr">
         <is>
-          <t>ADLQ-AG-0-0-T5/000SAN00M0</t>
+          <t>JN-A-0-D-N0/350x250/N/00/000</t>
         </is>
       </c>
       <c r="H15" s="33" t="n">
-        <v>76169900</v>
+        <v>90261029</v>
       </c>
       <c r="I15" s="46" t="n">
-        <v>218.87</v>
+        <v>236.06</v>
       </c>
       <c r="J15" s="35" t="n">
         <v>0</v>
       </c>
       <c r="K15" s="35" t="n">
-        <v>0.0325</v>
+        <v>0</v>
       </c>
       <c r="L15" s="36">
         <f>IF($H$4="-",0,IF($H$4="VAREJO",AW15,IF($H$4="ATACADO",AX15,0)))</f>
@@ -10792,12 +10790,12 @@
       </c>
       <c r="D16" s="33" t="inlineStr">
         <is>
-          <t>010 DIFUSOR ADLQ T4MM AG 0 AN0 TROX</t>
+          <t>010 DAMPER RG-B 200x155 TROX</t>
         </is>
       </c>
       <c r="E16" s="33" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>C</t>
         </is>
       </c>
       <c r="F16" s="71">
@@ -10806,20 +10804,20 @@
       </c>
       <c r="G16" s="33" t="inlineStr">
         <is>
-          <t>ADLQ-AG-0-0-T4/000SAN00M0</t>
+          <t>RG-B-200x155/D/0/00/000</t>
         </is>
       </c>
       <c r="H16" s="33" t="n">
-        <v>76169900</v>
+        <v>90261029</v>
       </c>
       <c r="I16" s="46" t="n">
-        <v>183.31</v>
+        <v>77.15000000000001</v>
       </c>
       <c r="J16" s="35" t="n">
         <v>0</v>
       </c>
       <c r="K16" s="35" t="n">
-        <v>0.0325</v>
+        <v>0</v>
       </c>
       <c r="L16" s="36">
         <f>IF($H$4="-",0,IF($H$4="VAREJO",AW16,IF($H$4="ATACADO",AX16,0)))</f>
@@ -10867,7 +10865,7 @@
         <v>7</v>
       </c>
       <c r="B17" s="33" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C17" s="33" t="inlineStr">
         <is>
@@ -10876,12 +10874,12 @@
       </c>
       <c r="D17" s="33" t="inlineStr">
         <is>
-          <t>010 DIFUSOR ADLQ T3MM AG 0 AN0 TROX</t>
+          <t>010 DAMPER JN-A 0 350x350 00 000 TROX</t>
         </is>
       </c>
       <c r="E17" s="33" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>C</t>
         </is>
       </c>
       <c r="F17" s="71">
@@ -10890,20 +10888,20 @@
       </c>
       <c r="G17" s="33" t="inlineStr">
         <is>
-          <t>ADLQ-AG-0-0-T3/000SAN00M0</t>
+          <t>JN-A-0-D-N0/350x350/N/00/000</t>
         </is>
       </c>
       <c r="H17" s="33" t="n">
-        <v>76169900</v>
+        <v>90261029</v>
       </c>
       <c r="I17" s="46" t="n">
-        <v>150.56</v>
+        <v>295.86</v>
       </c>
       <c r="J17" s="35" t="n">
         <v>0</v>
       </c>
       <c r="K17" s="35" t="n">
-        <v>0.0325</v>
+        <v>0</v>
       </c>
       <c r="L17" s="36">
         <f>IF($H$4="-",0,IF($H$4="VAREJO",AW17,IF($H$4="ATACADO",AX17,0)))</f>
@@ -10951,7 +10949,7 @@
         <v>8</v>
       </c>
       <c r="B18" s="33" t="n">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="C18" s="33" t="inlineStr">
         <is>
@@ -10960,7 +10958,7 @@
       </c>
       <c r="D18" s="33" t="inlineStr">
         <is>
-          <t>010 DIFUSOR ADLQ T2MM AG 0 AN0 TROX</t>
+          <t>010 GRELHA VAT-D 405x200 TROX</t>
         </is>
       </c>
       <c r="E18" s="33" t="inlineStr">
@@ -10974,14 +10972,14 @@
       </c>
       <c r="G18" s="33" t="inlineStr">
         <is>
-          <t>ADLQ-AG-0-0-T2/000SAN00M0</t>
+          <t>VAT-0-D405x200/00FAN0M0</t>
         </is>
       </c>
       <c r="H18" s="33" t="n">
         <v>76169900</v>
       </c>
       <c r="I18" s="46" t="n">
-        <v>114.13</v>
+        <v>125.87</v>
       </c>
       <c r="J18" s="35" t="n">
         <v>0</v>
@@ -11035,7 +11033,7 @@
         <v>9</v>
       </c>
       <c r="B19" s="33" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="C19" s="33" t="inlineStr">
         <is>
@@ -11044,7 +11042,7 @@
       </c>
       <c r="D19" s="33" t="inlineStr">
         <is>
-          <t>010 GRELHA VAT-AG 525x825 TROX</t>
+          <t>010 GRELHA VAT-D 505x250 TROX</t>
         </is>
       </c>
       <c r="E19" s="33" t="inlineStr">
@@ -11058,14 +11056,14 @@
       </c>
       <c r="G19" s="33" t="inlineStr">
         <is>
-          <t>VAT-0-AG525x825/00FAN0M0</t>
+          <t>VAT-0-D505x250/00FAN0M0</t>
         </is>
       </c>
       <c r="H19" s="33" t="n">
         <v>76169900</v>
       </c>
       <c r="I19" s="46" t="n">
-        <v>324.62</v>
+        <v>159.9</v>
       </c>
       <c r="J19" s="35" t="n">
         <v>0</v>
@@ -11119,7 +11117,7 @@
         <v>10</v>
       </c>
       <c r="B20" s="33" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C20" s="33" t="inlineStr">
         <is>
@@ -11128,7 +11126,7 @@
       </c>
       <c r="D20" s="33" t="inlineStr">
         <is>
-          <t>010 GRELHA VAT-AG 225x425 TROX</t>
+          <t>010 GRELHA VAT-D 145x150 TROX</t>
         </is>
       </c>
       <c r="E20" s="33" t="inlineStr">
@@ -11142,14 +11140,14 @@
       </c>
       <c r="G20" s="33" t="inlineStr">
         <is>
-          <t>VAT-0-AG225x425/00FAN0M0</t>
+          <t>VAT-0-D145x150/00FAN0M0</t>
         </is>
       </c>
       <c r="H20" s="33" t="n">
         <v>76169900</v>
       </c>
       <c r="I20" s="46" t="n">
-        <v>122.52</v>
+        <v>65.59999999999999</v>
       </c>
       <c r="J20" s="35" t="n">
         <v>0</v>
@@ -11203,7 +11201,7 @@
         <v>11</v>
       </c>
       <c r="B21" s="33" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C21" s="33" t="inlineStr">
         <is>
@@ -11212,12 +11210,12 @@
       </c>
       <c r="D21" s="33" t="inlineStr">
         <is>
-          <t>010 GRELHA VAT-AG 225x225 TROX</t>
+          <t>010 DAMPER JN-A 0 800x400 00 000 TROX</t>
         </is>
       </c>
       <c r="E21" s="33" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>C</t>
         </is>
       </c>
       <c r="F21" s="71">
@@ -11226,20 +11224,20 @@
       </c>
       <c r="G21" s="33" t="inlineStr">
         <is>
-          <t>VAT-0-AG225x225/00FAN0M0</t>
+          <t>JN-A-0-D-N0/800x400/N/00/000</t>
         </is>
       </c>
       <c r="H21" s="33" t="n">
-        <v>76169900</v>
+        <v>90261029</v>
       </c>
       <c r="I21" s="46" t="n">
-        <v>96.45</v>
+        <v>451.44</v>
       </c>
       <c r="J21" s="35" t="n">
         <v>0</v>
       </c>
       <c r="K21" s="35" t="n">
-        <v>0.0325</v>
+        <v>0</v>
       </c>
       <c r="L21" s="36">
         <f>IF($H$4="-",0,IF($H$4="VAREJO",AW21,IF($H$4="ATACADO",AX21,0)))</f>
@@ -11296,12 +11294,12 @@
       </c>
       <c r="D22" s="33" t="inlineStr">
         <is>
-          <t>010 GRELHA VAT-DG 125x325 TROX</t>
+          <t>010 DAMPER JN-A 0 300x200 00 000 TROX</t>
         </is>
       </c>
       <c r="E22" s="33" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>C</t>
         </is>
       </c>
       <c r="F22" s="71">
@@ -11310,20 +11308,20 @@
       </c>
       <c r="G22" s="33" t="inlineStr">
         <is>
-          <t>VAT-0-DG125x325/00FAN0M0</t>
+          <t>JN-A-0-D-N0/300x200/N/00/000</t>
         </is>
       </c>
       <c r="H22" s="33" t="n">
-        <v>76169900</v>
+        <v>90261029</v>
       </c>
       <c r="I22" s="46" t="n">
-        <v>96.87</v>
+        <v>195.91</v>
       </c>
       <c r="J22" s="35" t="n">
         <v>0</v>
       </c>
       <c r="K22" s="35" t="n">
-        <v>0.0325</v>
+        <v>0</v>
       </c>
       <c r="L22" s="36">
         <f>IF($H$4="-",0,IF($H$4="VAREJO",AW22,IF($H$4="ATACADO",AX22,0)))</f>
@@ -11380,12 +11378,12 @@
       </c>
       <c r="D23" s="33" t="inlineStr">
         <is>
-          <t>010 GRELHA AT-DG 325x85 TROX</t>
+          <t>010 DAMPER RG-B 300x105 TROX</t>
         </is>
       </c>
       <c r="E23" s="33" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>C</t>
         </is>
       </c>
       <c r="F23" s="71">
@@ -11394,20 +11392,20 @@
       </c>
       <c r="G23" s="33" t="inlineStr">
         <is>
-          <t>AT-0-DG325x85/00FAN0M0</t>
+          <t>RG-B-300x105/D/0/00/000</t>
         </is>
       </c>
       <c r="H23" s="33" t="n">
-        <v>76169900</v>
+        <v>90261029</v>
       </c>
       <c r="I23" s="46" t="n">
-        <v>96.97</v>
+        <v>77.29000000000001</v>
       </c>
       <c r="J23" s="35" t="n">
         <v>0</v>
       </c>
       <c r="K23" s="35" t="n">
-        <v>0.0325</v>
+        <v>0</v>
       </c>
       <c r="L23" s="36">
         <f>IF($H$4="-",0,IF($H$4="VAREJO",AW23,IF($H$4="ATACADO",AX23,0)))</f>
@@ -11455,7 +11453,7 @@
         <v>14</v>
       </c>
       <c r="B24" s="33" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C24" s="33" t="inlineStr">
         <is>
@@ -11464,7 +11462,7 @@
       </c>
       <c r="D24" s="33" t="inlineStr">
         <is>
-          <t>010 VENEZIANA AWK 397x197 AN0 TROX</t>
+          <t>010 DAMPER RG-B 300x155 TROX</t>
         </is>
       </c>
       <c r="E24" s="33" t="inlineStr">
@@ -11478,20 +11476,20 @@
       </c>
       <c r="G24" s="33" t="inlineStr">
         <is>
-          <t>AWK/397x197/0/0/F/AN0/0</t>
+          <t>RG-B-300x155/D/0/00/000</t>
         </is>
       </c>
       <c r="H24" s="33" t="n">
-        <v>76169900</v>
+        <v>90261029</v>
       </c>
       <c r="I24" s="46" t="n">
-        <v>84.95999999999999</v>
+        <v>88.16</v>
       </c>
       <c r="J24" s="35" t="n">
         <v>0</v>
       </c>
       <c r="K24" s="35" t="n">
-        <v>0.0325</v>
+        <v>0</v>
       </c>
       <c r="L24" s="36">
         <f>IF($H$4="-",0,IF($H$4="VAREJO",AW24,IF($H$4="ATACADO",AX24,0)))</f>
@@ -11539,7 +11537,7 @@
         <v>15</v>
       </c>
       <c r="B25" s="33" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C25" s="33" t="inlineStr">
         <is>
@@ -11548,12 +11546,12 @@
       </c>
       <c r="D25" s="33" t="inlineStr">
         <is>
-          <t>010 VENEZIANA AWK 297x197 AN0 TROX</t>
+          <t>010 GRELHA AR-AG 150x145 AN0 TROX</t>
         </is>
       </c>
       <c r="E25" s="33" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>A</t>
         </is>
       </c>
       <c r="F25" s="71">
@@ -11562,14 +11560,14 @@
       </c>
       <c r="G25" s="33" t="inlineStr">
         <is>
-          <t>AWK/297x197/0/0/F/AN0/0</t>
+          <t>AR-AG-150x145/0/0/FAN0M0</t>
         </is>
       </c>
       <c r="H25" s="33" t="n">
         <v>76169900</v>
       </c>
       <c r="I25" s="46" t="n">
-        <v>72.73999999999999</v>
+        <v>70.01000000000001</v>
       </c>
       <c r="J25" s="35" t="n">
         <v>0</v>
@@ -11623,7 +11621,7 @@
         <v>16</v>
       </c>
       <c r="B26" s="33" t="n">
-        <v>1</v>
+        <v>29</v>
       </c>
       <c r="C26" s="33" t="inlineStr">
         <is>
@@ -11632,12 +11630,12 @@
       </c>
       <c r="D26" s="33" t="inlineStr">
         <is>
-          <t>010 DAMPER RG-B 250x155 TROX</t>
+          <t>010 GRELHA AR-AG 250x205 AN0 TROX</t>
         </is>
       </c>
       <c r="E26" s="33" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>A</t>
         </is>
       </c>
       <c r="F26" s="71">
@@ -11646,20 +11644,20 @@
       </c>
       <c r="G26" s="33" t="inlineStr">
         <is>
-          <t>RG-B-250x155/D/0/00/000</t>
+          <t>AR-AG-250x205/0/0/FAN0M0</t>
         </is>
       </c>
       <c r="H26" s="33" t="n">
-        <v>90261029</v>
+        <v>76169900</v>
       </c>
       <c r="I26" s="46" t="n">
-        <v>85.13</v>
+        <v>95.22</v>
       </c>
       <c r="J26" s="35" t="n">
         <v>0</v>
       </c>
       <c r="K26" s="35" t="n">
-        <v>0</v>
+        <v>0.0325</v>
       </c>
       <c r="L26" s="36">
         <f>IF($H$4="-",0,IF($H$4="VAREJO",AW26,IF($H$4="ATACADO",AX26,0)))</f>
@@ -11707,7 +11705,7 @@
         <v>17</v>
       </c>
       <c r="B27" s="33" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C27" s="33" t="inlineStr">
         <is>
@@ -11716,7 +11714,7 @@
       </c>
       <c r="D27" s="33" t="inlineStr">
         <is>
-          <t>010 DAMPER RG-B 500x405 TROX</t>
+          <t>010 TOMADA DE AR VDF F711 AWK 947x797  TROX</t>
         </is>
       </c>
       <c r="E27" s="33" t="inlineStr">
@@ -11730,20 +11728,20 @@
       </c>
       <c r="G27" s="33" t="inlineStr">
         <is>
-          <t>RG-B-500x405/D/0/00/000</t>
+          <t>VDF-F711/947x797/K/AG/F/AN0</t>
         </is>
       </c>
       <c r="H27" s="33" t="n">
-        <v>90261029</v>
+        <v>76169900</v>
       </c>
       <c r="I27" s="46" t="n">
-        <v>182.05</v>
+        <v>625.96</v>
       </c>
       <c r="J27" s="35" t="n">
         <v>0</v>
       </c>
       <c r="K27" s="35" t="n">
-        <v>0</v>
+        <v>0.0325</v>
       </c>
       <c r="L27" s="36">
         <f>IF($H$4="-",0,IF($H$4="VAREJO",AW27,IF($H$4="ATACADO",AX27,0)))</f>
@@ -11800,7 +11798,7 @@
       </c>
       <c r="D28" s="33" t="inlineStr">
         <is>
-          <t>010 DAMPER RG-B 400x155 TROX</t>
+          <t>010 DAMPER JN-A 0 800x400 00 000 TROX</t>
         </is>
       </c>
       <c r="E28" s="33" t="inlineStr">
@@ -11814,14 +11812,14 @@
       </c>
       <c r="G28" s="33" t="inlineStr">
         <is>
-          <t>RG-B-400x155/D/0/00/000</t>
+          <t>JN-A-0-D-N0/800x400/N/00/000</t>
         </is>
       </c>
       <c r="H28" s="33" t="n">
         <v>90261029</v>
       </c>
       <c r="I28" s="46" t="n">
-        <v>102.14</v>
+        <v>451.44</v>
       </c>
       <c r="J28" s="35" t="n">
         <v>0</v>
@@ -11884,7 +11882,7 @@
       </c>
       <c r="D29" s="33" t="inlineStr">
         <is>
-          <t>010 DAMPER RG-B 500x205 TROX</t>
+          <t>010 DAMPER JN-A 0 500x300 00 000 TROX</t>
         </is>
       </c>
       <c r="E29" s="33" t="inlineStr">
@@ -11898,14 +11896,14 @@
       </c>
       <c r="G29" s="33" t="inlineStr">
         <is>
-          <t>RG-B-500x205/D/0/00/000</t>
+          <t>JN-A-0-D-N0/500x300/N/00/000</t>
         </is>
       </c>
       <c r="H29" s="33" t="n">
         <v>90261029</v>
       </c>
       <c r="I29" s="46" t="n">
-        <v>127.2</v>
+        <v>302.27</v>
       </c>
       <c r="J29" s="35" t="n">
         <v>0</v>
@@ -11968,7 +11966,7 @@
       </c>
       <c r="D30" s="33" t="inlineStr">
         <is>
-          <t>010 DAMPER RG-B 500x205 TROX</t>
+          <t>010 DAMPER RG-B 300x155 TROX</t>
         </is>
       </c>
       <c r="E30" s="33" t="inlineStr">
@@ -11982,14 +11980,14 @@
       </c>
       <c r="G30" s="33" t="inlineStr">
         <is>
-          <t>RG-B-500x205/D/0/00/000</t>
+          <t>RG-B-300x155/D/0/00/000</t>
         </is>
       </c>
       <c r="H30" s="33" t="n">
         <v>90261029</v>
       </c>
       <c r="I30" s="46" t="n">
-        <v>127.2</v>
+        <v>88.16</v>
       </c>
       <c r="J30" s="35" t="n">
         <v>0</v>
@@ -12043,7 +12041,7 @@
         <v>21</v>
       </c>
       <c r="B31" s="33" t="n">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="C31" s="33" t="inlineStr">
         <is>
@@ -12052,12 +12050,12 @@
       </c>
       <c r="D31" s="33" t="inlineStr">
         <is>
-          <t>010 DAMPER RG-B 200x205 TROX</t>
+          <t>010 GRELHA VAT-DG 405x400 TROX</t>
         </is>
       </c>
       <c r="E31" s="33" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>B</t>
         </is>
       </c>
       <c r="F31" s="71">
@@ -12066,20 +12064,20 @@
       </c>
       <c r="G31" s="33" t="inlineStr">
         <is>
-          <t>RG-B-200x205/D/0/00/000</t>
+          <t>VAT-0-DG405x400/00FAN0M0</t>
         </is>
       </c>
       <c r="H31" s="33" t="n">
-        <v>90261029</v>
+        <v>76169900</v>
       </c>
       <c r="I31" s="46" t="n">
-        <v>89.41</v>
+        <v>218.19</v>
       </c>
       <c r="J31" s="35" t="n">
         <v>0</v>
       </c>
       <c r="K31" s="35" t="n">
-        <v>0</v>
+        <v>0.0325</v>
       </c>
       <c r="L31" s="36">
         <f>IF($H$4="-",0,IF($H$4="VAREJO",AW31,IF($H$4="ATACADO",AX31,0)))</f>
@@ -12127,7 +12125,7 @@
         <v>22</v>
       </c>
       <c r="B32" s="33" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C32" s="33" t="inlineStr">
         <is>
@@ -12136,12 +12134,12 @@
       </c>
       <c r="D32" s="33" t="inlineStr">
         <is>
-          <t>010 DAMPER RG-B 300x105 TROX</t>
+          <t>010 GRELHA VAT-DG 245x250 TROX</t>
         </is>
       </c>
       <c r="E32" s="33" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>A</t>
         </is>
       </c>
       <c r="F32" s="71">
@@ -12150,20 +12148,20 @@
       </c>
       <c r="G32" s="33" t="inlineStr">
         <is>
-          <t>RG-B-300x105/D/0/00/000</t>
+          <t>VAT-0-DG245x250/00FAN0M0</t>
         </is>
       </c>
       <c r="H32" s="33" t="n">
-        <v>90261029</v>
+        <v>76169900</v>
       </c>
       <c r="I32" s="46" t="n">
-        <v>79.59999999999999</v>
+        <v>123.44</v>
       </c>
       <c r="J32" s="35" t="n">
         <v>0</v>
       </c>
       <c r="K32" s="35" t="n">
-        <v>0</v>
+        <v>0.0325</v>
       </c>
       <c r="L32" s="36">
         <f>IF($H$4="-",0,IF($H$4="VAREJO",AW32,IF($H$4="ATACADO",AX32,0)))</f>
@@ -12220,7 +12218,7 @@
       </c>
       <c r="D33" s="33" t="inlineStr">
         <is>
-          <t>010 DAMPER RG-B 300x205 TROX</t>
+          <t>010 DAMPER RG-B 250x155 TROX</t>
         </is>
       </c>
       <c r="E33" s="33" t="inlineStr">
@@ -12234,14 +12232,14 @@
       </c>
       <c r="G33" s="33" t="inlineStr">
         <is>
-          <t>RG-B-300x205/D/0/00/000</t>
+          <t>RG-B-250x155/D/0/00/000</t>
         </is>
       </c>
       <c r="H33" s="33" t="n">
         <v>90261029</v>
       </c>
       <c r="I33" s="46" t="n">
-        <v>102</v>
+        <v>82.65000000000001</v>
       </c>
       <c r="J33" s="35" t="n">
         <v>0</v>
@@ -12294,45 +12292,23 @@
       <c r="A34" s="32" t="n">
         <v>24</v>
       </c>
-      <c r="B34" s="33" t="n">
-        <v>1</v>
-      </c>
-      <c r="C34" s="33" t="inlineStr">
-        <is>
-          <t>PÇ</t>
-        </is>
-      </c>
-      <c r="D34" s="33" t="inlineStr">
-        <is>
-          <t>010 DAMPER RG-B 600x405 TROX</t>
-        </is>
-      </c>
+      <c r="B34" s="33" t="n"/>
+      <c r="C34" s="33" t="n"/>
+      <c r="D34" s="33" t="n"/>
       <c r="E34" s="33" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>-</t>
         </is>
       </c>
       <c r="F34" s="71">
         <f>IFERROR((VLOOKUP(E34,$AE$11:$AG$14,3,0)),"-")</f>
         <v/>
       </c>
-      <c r="G34" s="33" t="inlineStr">
-        <is>
-          <t>RG-B-600x405/D/0/00/000</t>
-        </is>
-      </c>
-      <c r="H34" s="33" t="n">
-        <v>90261029</v>
-      </c>
-      <c r="I34" s="46" t="n">
-        <v>199.67</v>
-      </c>
-      <c r="J34" s="35" t="n">
-        <v>0</v>
-      </c>
-      <c r="K34" s="35" t="n">
-        <v>0</v>
-      </c>
+      <c r="G34" s="33" t="n"/>
+      <c r="H34" s="33" t="n"/>
+      <c r="I34" s="46" t="n"/>
+      <c r="J34" s="35" t="n"/>
+      <c r="K34" s="35" t="n"/>
       <c r="L34" s="36">
         <f>IF($H$4="-",0,IF($H$4="VAREJO",AW34,IF($H$4="ATACADO",AX34,0)))</f>
         <v/>
@@ -12378,45 +12354,23 @@
       <c r="A35" s="32" t="n">
         <v>25</v>
       </c>
-      <c r="B35" s="33" t="n">
-        <v>1</v>
-      </c>
-      <c r="C35" s="33" t="inlineStr">
-        <is>
-          <t>PÇ</t>
-        </is>
-      </c>
-      <c r="D35" s="33" t="inlineStr">
-        <is>
-          <t>010 DAMPER RG-B 300x155 TROX</t>
-        </is>
-      </c>
+      <c r="B35" s="33" t="n"/>
+      <c r="C35" s="33" t="n"/>
+      <c r="D35" s="33" t="n"/>
       <c r="E35" s="33" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>-</t>
         </is>
       </c>
       <c r="F35" s="71">
         <f>IFERROR((VLOOKUP(E35,$AE$11:$AG$14,3,0)),"-")</f>
         <v/>
       </c>
-      <c r="G35" s="33" t="inlineStr">
-        <is>
-          <t>RG-B-300x155/D/0/00/000</t>
-        </is>
-      </c>
-      <c r="H35" s="33" t="n">
-        <v>90261029</v>
-      </c>
-      <c r="I35" s="46" t="n">
-        <v>90.8</v>
-      </c>
-      <c r="J35" s="35" t="n">
-        <v>0</v>
-      </c>
-      <c r="K35" s="35" t="n">
-        <v>0</v>
-      </c>
+      <c r="G35" s="33" t="n"/>
+      <c r="H35" s="33" t="n"/>
+      <c r="I35" s="46" t="n"/>
+      <c r="J35" s="35" t="n"/>
+      <c r="K35" s="35" t="n"/>
       <c r="L35" s="36">
         <f>IF($H$4="-",0,IF($H$4="VAREJO",AW35,IF($H$4="ATACADO",AX35,0)))</f>
         <v/>
@@ -12462,45 +12416,23 @@
       <c r="A36" s="32" t="n">
         <v>26</v>
       </c>
-      <c r="B36" s="33" t="n">
-        <v>1</v>
-      </c>
-      <c r="C36" s="33" t="inlineStr">
-        <is>
-          <t>PÇ</t>
-        </is>
-      </c>
-      <c r="D36" s="33" t="inlineStr">
-        <is>
-          <t>010 DAMPER RG-B 200x105 TROX</t>
-        </is>
-      </c>
+      <c r="B36" s="33" t="n"/>
+      <c r="C36" s="33" t="n"/>
+      <c r="D36" s="33" t="n"/>
       <c r="E36" s="33" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>-</t>
         </is>
       </c>
       <c r="F36" s="71">
         <f>IFERROR((VLOOKUP(E36,$AE$11:$AG$14,3,0)),"-")</f>
         <v/>
       </c>
-      <c r="G36" s="33" t="inlineStr">
-        <is>
-          <t>RG-B-200x105/D/0/00/000</t>
-        </is>
-      </c>
-      <c r="H36" s="33" t="n">
-        <v>90261029</v>
-      </c>
-      <c r="I36" s="46" t="n">
-        <v>69.52</v>
-      </c>
-      <c r="J36" s="35" t="n">
-        <v>0</v>
-      </c>
-      <c r="K36" s="35" t="n">
-        <v>0</v>
-      </c>
+      <c r="G36" s="33" t="n"/>
+      <c r="H36" s="33" t="n"/>
+      <c r="I36" s="46" t="n"/>
+      <c r="J36" s="35" t="n"/>
+      <c r="K36" s="35" t="n"/>
       <c r="L36" s="36">
         <f>IF($H$4="-",0,IF($H$4="VAREJO",AW36,IF($H$4="ATACADO",AX36,0)))</f>
         <v/>

</xml_diff>

<commit_message>
novo modelo de composição
</commit_message>
<xml_diff>
--- a/PlanDist.xlsx
+++ b/PlanDist.xlsx
@@ -9938,7 +9938,7 @@
       <c r="B3" s="111" t="n"/>
       <c r="C3" s="112" t="inlineStr">
         <is>
-          <t>Felipe Almeida</t>
+          <t>Luiz Henrique</t>
         </is>
       </c>
       <c r="D3" s="113" t="n"/>
@@ -9968,7 +9968,7 @@
       <c r="B4" s="111" t="n"/>
       <c r="C4" s="112" t="inlineStr">
         <is>
-          <t>Wellisson Chaves</t>
+          <t>Larissa Sousa</t>
         </is>
       </c>
       <c r="D4" s="113" t="n"/>
@@ -9994,7 +9994,7 @@
       <c r="B5" s="111" t="n"/>
       <c r="C5" s="76" t="inlineStr">
         <is>
-          <t>1020</t>
+          <t>1026</t>
         </is>
       </c>
       <c r="E5" s="21" t="n"/>
@@ -10229,7 +10229,7 @@
         <v>1</v>
       </c>
       <c r="B11" s="33" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C11" s="33" t="inlineStr">
         <is>
@@ -10238,7 +10238,7 @@
       </c>
       <c r="D11" s="33" t="inlineStr">
         <is>
-          <t>010 TOMADA DE AR VDF F711 AWG 597x597  TROX</t>
+          <t>010 DIFUSOR VSD 35 4 1200 0 F AN0 TROX</t>
         </is>
       </c>
       <c r="E11" s="33" t="inlineStr">
@@ -10252,14 +10252,14 @@
       </c>
       <c r="G11" s="33" t="inlineStr">
         <is>
-          <t>VDF-F711/597x597/G/AG/F/AN0</t>
+          <t>VSD35-4F01200x0x00000AN0</t>
         </is>
       </c>
       <c r="H11" s="33" t="n">
         <v>76169900</v>
       </c>
       <c r="I11" s="34" t="n">
-        <v>488.82</v>
+        <v>247.64</v>
       </c>
       <c r="J11" s="35" t="n">
         <v>0</v>
@@ -10345,45 +10345,23 @@
       <c r="A12" s="32" t="n">
         <v>2</v>
       </c>
-      <c r="B12" s="33" t="n">
-        <v>2</v>
-      </c>
-      <c r="C12" s="33" t="inlineStr">
-        <is>
-          <t>PÇ</t>
-        </is>
-      </c>
-      <c r="D12" s="33" t="inlineStr">
-        <is>
-          <t>010 TOMADA DE AR VDF F711 AWG 497x497  TROX</t>
-        </is>
-      </c>
+      <c r="B12" s="33" t="n"/>
+      <c r="C12" s="33" t="n"/>
+      <c r="D12" s="33" t="n"/>
       <c r="E12" s="33" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>-</t>
         </is>
       </c>
       <c r="F12" s="71">
         <f>IFERROR((VLOOKUP(E12,$AE$11:$AG$14,3,0)),"-")</f>
         <v/>
       </c>
-      <c r="G12" s="33" t="inlineStr">
-        <is>
-          <t>VDF-F711/497x497/G/AG/F/AN0</t>
-        </is>
-      </c>
-      <c r="H12" s="33" t="n">
-        <v>76169900</v>
-      </c>
-      <c r="I12" s="46" t="n">
-        <v>405.67</v>
-      </c>
-      <c r="J12" s="35" t="n">
-        <v>0</v>
-      </c>
-      <c r="K12" s="35" t="n">
-        <v>0.0325</v>
-      </c>
+      <c r="G12" s="33" t="n"/>
+      <c r="H12" s="33" t="n"/>
+      <c r="I12" s="46" t="n"/>
+      <c r="J12" s="35" t="n"/>
+      <c r="K12" s="35" t="n"/>
       <c r="L12" s="36">
         <f>IF($H$4="-",0,IF($H$4="VAREJO",AW12,IF($H$4="ATACADO",AX12,0)))</f>
         <v/>
@@ -10462,45 +10440,23 @@
       <c r="A13" s="32" t="n">
         <v>3</v>
       </c>
-      <c r="B13" s="33" t="n">
-        <v>1</v>
-      </c>
-      <c r="C13" s="33" t="inlineStr">
-        <is>
-          <t>PÇ</t>
-        </is>
-      </c>
-      <c r="D13" s="33" t="inlineStr">
-        <is>
-          <t>010 DAMPER JN-A 0 700x250 00 000 TROX</t>
-        </is>
-      </c>
+      <c r="B13" s="33" t="n"/>
+      <c r="C13" s="33" t="n"/>
+      <c r="D13" s="33" t="n"/>
       <c r="E13" s="33" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>-</t>
         </is>
       </c>
       <c r="F13" s="71">
         <f>IFERROR((VLOOKUP(E13,$AE$11:$AG$14,3,0)),"-")</f>
         <v/>
       </c>
-      <c r="G13" s="33" t="inlineStr">
-        <is>
-          <t>JN-A-0-D-N0/700x250/N/00/000</t>
-        </is>
-      </c>
-      <c r="H13" s="33" t="n">
-        <v>90261029</v>
-      </c>
-      <c r="I13" s="46" t="n">
-        <v>314.28</v>
-      </c>
-      <c r="J13" s="35" t="n">
-        <v>0</v>
-      </c>
-      <c r="K13" s="35" t="n">
-        <v>0</v>
-      </c>
+      <c r="G13" s="33" t="n"/>
+      <c r="H13" s="33" t="n"/>
+      <c r="I13" s="46" t="n"/>
+      <c r="J13" s="35" t="n"/>
+      <c r="K13" s="35" t="n"/>
       <c r="L13" s="36">
         <f>IF($H$4="-",0,IF($H$4="VAREJO",AW13,IF($H$4="ATACADO",AX13,0)))</f>
         <v/>
@@ -10579,45 +10535,23 @@
       <c r="A14" s="32" t="n">
         <v>4</v>
       </c>
-      <c r="B14" s="33" t="n">
-        <v>1</v>
-      </c>
-      <c r="C14" s="33" t="inlineStr">
-        <is>
-          <t>PÇ</t>
-        </is>
-      </c>
-      <c r="D14" s="33" t="inlineStr">
-        <is>
-          <t>010 DAMPER JN-A 0 400x250 00 000 TROX</t>
-        </is>
-      </c>
+      <c r="B14" s="33" t="n"/>
+      <c r="C14" s="33" t="n"/>
+      <c r="D14" s="33" t="n"/>
       <c r="E14" s="33" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>-</t>
         </is>
       </c>
       <c r="F14" s="71">
         <f>IFERROR((VLOOKUP(E14,$AE$11:$AG$14,3,0)),"-")</f>
         <v/>
       </c>
-      <c r="G14" s="33" t="inlineStr">
-        <is>
-          <t>JN-A-0-D-N0/400x250/N/00/000</t>
-        </is>
-      </c>
-      <c r="H14" s="33" t="n">
-        <v>90261029</v>
-      </c>
-      <c r="I14" s="46" t="n">
-        <v>247.23</v>
-      </c>
-      <c r="J14" s="35" t="n">
-        <v>0</v>
-      </c>
-      <c r="K14" s="35" t="n">
-        <v>0</v>
-      </c>
+      <c r="G14" s="33" t="n"/>
+      <c r="H14" s="33" t="n"/>
+      <c r="I14" s="46" t="n"/>
+      <c r="J14" s="35" t="n"/>
+      <c r="K14" s="35" t="n"/>
       <c r="L14" s="36">
         <f>IF($H$4="-",0,IF($H$4="VAREJO",AW14,IF($H$4="ATACADO",AX14,0)))</f>
         <v/>
@@ -10696,45 +10630,23 @@
       <c r="A15" s="32" t="n">
         <v>5</v>
       </c>
-      <c r="B15" s="33" t="n">
-        <v>1</v>
-      </c>
-      <c r="C15" s="33" t="inlineStr">
-        <is>
-          <t>PÇ</t>
-        </is>
-      </c>
-      <c r="D15" s="33" t="inlineStr">
-        <is>
-          <t>010 DAMPER JN-A 0 350x250 00 000 TROX</t>
-        </is>
-      </c>
+      <c r="B15" s="33" t="n"/>
+      <c r="C15" s="33" t="n"/>
+      <c r="D15" s="33" t="n"/>
       <c r="E15" s="33" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>-</t>
         </is>
       </c>
       <c r="F15" s="71">
         <f>IFERROR((VLOOKUP(E15,$AE$11:$AG$14,3,0)),"-")</f>
         <v/>
       </c>
-      <c r="G15" s="33" t="inlineStr">
-        <is>
-          <t>JN-A-0-D-N0/350x250/N/00/000</t>
-        </is>
-      </c>
-      <c r="H15" s="33" t="n">
-        <v>90261029</v>
-      </c>
-      <c r="I15" s="46" t="n">
-        <v>236.06</v>
-      </c>
-      <c r="J15" s="35" t="n">
-        <v>0</v>
-      </c>
-      <c r="K15" s="35" t="n">
-        <v>0</v>
-      </c>
+      <c r="G15" s="33" t="n"/>
+      <c r="H15" s="33" t="n"/>
+      <c r="I15" s="46" t="n"/>
+      <c r="J15" s="35" t="n"/>
+      <c r="K15" s="35" t="n"/>
       <c r="L15" s="36">
         <f>IF($H$4="-",0,IF($H$4="VAREJO",AW15,IF($H$4="ATACADO",AX15,0)))</f>
         <v/>
@@ -10780,45 +10692,23 @@
       <c r="A16" s="32" t="n">
         <v>6</v>
       </c>
-      <c r="B16" s="33" t="n">
-        <v>1</v>
-      </c>
-      <c r="C16" s="33" t="inlineStr">
-        <is>
-          <t>PÇ</t>
-        </is>
-      </c>
-      <c r="D16" s="33" t="inlineStr">
-        <is>
-          <t>010 DAMPER RG-B 200x155 TROX</t>
-        </is>
-      </c>
+      <c r="B16" s="33" t="n"/>
+      <c r="C16" s="33" t="n"/>
+      <c r="D16" s="33" t="n"/>
       <c r="E16" s="33" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>-</t>
         </is>
       </c>
       <c r="F16" s="71">
         <f>IFERROR((VLOOKUP(E16,$AE$11:$AG$14,3,0)),"-")</f>
         <v/>
       </c>
-      <c r="G16" s="33" t="inlineStr">
-        <is>
-          <t>RG-B-200x155/D/0/00/000</t>
-        </is>
-      </c>
-      <c r="H16" s="33" t="n">
-        <v>90261029</v>
-      </c>
-      <c r="I16" s="46" t="n">
-        <v>77.15000000000001</v>
-      </c>
-      <c r="J16" s="35" t="n">
-        <v>0</v>
-      </c>
-      <c r="K16" s="35" t="n">
-        <v>0</v>
-      </c>
+      <c r="G16" s="33" t="n"/>
+      <c r="H16" s="33" t="n"/>
+      <c r="I16" s="46" t="n"/>
+      <c r="J16" s="35" t="n"/>
+      <c r="K16" s="35" t="n"/>
       <c r="L16" s="36">
         <f>IF($H$4="-",0,IF($H$4="VAREJO",AW16,IF($H$4="ATACADO",AX16,0)))</f>
         <v/>
@@ -10864,45 +10754,23 @@
       <c r="A17" s="32" t="n">
         <v>7</v>
       </c>
-      <c r="B17" s="33" t="n">
-        <v>1</v>
-      </c>
-      <c r="C17" s="33" t="inlineStr">
-        <is>
-          <t>PÇ</t>
-        </is>
-      </c>
-      <c r="D17" s="33" t="inlineStr">
-        <is>
-          <t>010 DAMPER JN-A 0 350x350 00 000 TROX</t>
-        </is>
-      </c>
+      <c r="B17" s="33" t="n"/>
+      <c r="C17" s="33" t="n"/>
+      <c r="D17" s="33" t="n"/>
       <c r="E17" s="33" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>-</t>
         </is>
       </c>
       <c r="F17" s="71">
         <f>IFERROR((VLOOKUP(E17,$AE$11:$AG$14,3,0)),"-")</f>
         <v/>
       </c>
-      <c r="G17" s="33" t="inlineStr">
-        <is>
-          <t>JN-A-0-D-N0/350x350/N/00/000</t>
-        </is>
-      </c>
-      <c r="H17" s="33" t="n">
-        <v>90261029</v>
-      </c>
-      <c r="I17" s="46" t="n">
-        <v>295.86</v>
-      </c>
-      <c r="J17" s="35" t="n">
-        <v>0</v>
-      </c>
-      <c r="K17" s="35" t="n">
-        <v>0</v>
-      </c>
+      <c r="G17" s="33" t="n"/>
+      <c r="H17" s="33" t="n"/>
+      <c r="I17" s="46" t="n"/>
+      <c r="J17" s="35" t="n"/>
+      <c r="K17" s="35" t="n"/>
       <c r="L17" s="36">
         <f>IF($H$4="-",0,IF($H$4="VAREJO",AW17,IF($H$4="ATACADO",AX17,0)))</f>
         <v/>
@@ -10948,45 +10816,23 @@
       <c r="A18" s="32" t="n">
         <v>8</v>
       </c>
-      <c r="B18" s="33" t="n">
-        <v>17</v>
-      </c>
-      <c r="C18" s="33" t="inlineStr">
-        <is>
-          <t>PÇ</t>
-        </is>
-      </c>
-      <c r="D18" s="33" t="inlineStr">
-        <is>
-          <t>010 GRELHA VAT-D 405x200 TROX</t>
-        </is>
-      </c>
+      <c r="B18" s="33" t="n"/>
+      <c r="C18" s="33" t="n"/>
+      <c r="D18" s="33" t="n"/>
       <c r="E18" s="33" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>-</t>
         </is>
       </c>
       <c r="F18" s="71">
         <f>IFERROR((VLOOKUP(E18,$AE$11:$AG$14,3,0)),"-")</f>
         <v/>
       </c>
-      <c r="G18" s="33" t="inlineStr">
-        <is>
-          <t>VAT-0-D405x200/00FAN0M0</t>
-        </is>
-      </c>
-      <c r="H18" s="33" t="n">
-        <v>76169900</v>
-      </c>
-      <c r="I18" s="46" t="n">
-        <v>125.87</v>
-      </c>
-      <c r="J18" s="35" t="n">
-        <v>0</v>
-      </c>
-      <c r="K18" s="35" t="n">
-        <v>0.0325</v>
-      </c>
+      <c r="G18" s="33" t="n"/>
+      <c r="H18" s="33" t="n"/>
+      <c r="I18" s="46" t="n"/>
+      <c r="J18" s="35" t="n"/>
+      <c r="K18" s="35" t="n"/>
       <c r="L18" s="36">
         <f>IF($H$4="-",0,IF($H$4="VAREJO",AW18,IF($H$4="ATACADO",AX18,0)))</f>
         <v/>
@@ -11032,45 +10878,23 @@
       <c r="A19" s="32" t="n">
         <v>9</v>
       </c>
-      <c r="B19" s="33" t="n">
-        <v>7</v>
-      </c>
-      <c r="C19" s="33" t="inlineStr">
-        <is>
-          <t>PÇ</t>
-        </is>
-      </c>
-      <c r="D19" s="33" t="inlineStr">
-        <is>
-          <t>010 GRELHA VAT-D 505x250 TROX</t>
-        </is>
-      </c>
+      <c r="B19" s="33" t="n"/>
+      <c r="C19" s="33" t="n"/>
+      <c r="D19" s="33" t="n"/>
       <c r="E19" s="33" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>-</t>
         </is>
       </c>
       <c r="F19" s="71">
         <f>IFERROR((VLOOKUP(E19,$AE$11:$AG$14,3,0)),"-")</f>
         <v/>
       </c>
-      <c r="G19" s="33" t="inlineStr">
-        <is>
-          <t>VAT-0-D505x250/00FAN0M0</t>
-        </is>
-      </c>
-      <c r="H19" s="33" t="n">
-        <v>76169900</v>
-      </c>
-      <c r="I19" s="46" t="n">
-        <v>159.9</v>
-      </c>
-      <c r="J19" s="35" t="n">
-        <v>0</v>
-      </c>
-      <c r="K19" s="35" t="n">
-        <v>0.0325</v>
-      </c>
+      <c r="G19" s="33" t="n"/>
+      <c r="H19" s="33" t="n"/>
+      <c r="I19" s="46" t="n"/>
+      <c r="J19" s="35" t="n"/>
+      <c r="K19" s="35" t="n"/>
       <c r="L19" s="36">
         <f>IF($H$4="-",0,IF($H$4="VAREJO",AW19,IF($H$4="ATACADO",AX19,0)))</f>
         <v/>
@@ -11116,45 +10940,23 @@
       <c r="A20" s="32" t="n">
         <v>10</v>
       </c>
-      <c r="B20" s="33" t="n">
-        <v>3</v>
-      </c>
-      <c r="C20" s="33" t="inlineStr">
-        <is>
-          <t>PÇ</t>
-        </is>
-      </c>
-      <c r="D20" s="33" t="inlineStr">
-        <is>
-          <t>010 GRELHA VAT-D 145x150 TROX</t>
-        </is>
-      </c>
+      <c r="B20" s="33" t="n"/>
+      <c r="C20" s="33" t="n"/>
+      <c r="D20" s="33" t="n"/>
       <c r="E20" s="33" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>-</t>
         </is>
       </c>
       <c r="F20" s="71">
         <f>IFERROR((VLOOKUP(E20,$AE$11:$AG$14,3,0)),"-")</f>
         <v/>
       </c>
-      <c r="G20" s="33" t="inlineStr">
-        <is>
-          <t>VAT-0-D145x150/00FAN0M0</t>
-        </is>
-      </c>
-      <c r="H20" s="33" t="n">
-        <v>76169900</v>
-      </c>
-      <c r="I20" s="46" t="n">
-        <v>65.59999999999999</v>
-      </c>
-      <c r="J20" s="35" t="n">
-        <v>0</v>
-      </c>
-      <c r="K20" s="35" t="n">
-        <v>0.0325</v>
-      </c>
+      <c r="G20" s="33" t="n"/>
+      <c r="H20" s="33" t="n"/>
+      <c r="I20" s="46" t="n"/>
+      <c r="J20" s="35" t="n"/>
+      <c r="K20" s="35" t="n"/>
       <c r="L20" s="36">
         <f>IF($H$4="-",0,IF($H$4="VAREJO",AW20,IF($H$4="ATACADO",AX20,0)))</f>
         <v/>
@@ -11200,45 +11002,23 @@
       <c r="A21" s="32" t="n">
         <v>11</v>
       </c>
-      <c r="B21" s="33" t="n">
-        <v>1</v>
-      </c>
-      <c r="C21" s="33" t="inlineStr">
-        <is>
-          <t>PÇ</t>
-        </is>
-      </c>
-      <c r="D21" s="33" t="inlineStr">
-        <is>
-          <t>010 DAMPER JN-A 0 800x400 00 000 TROX</t>
-        </is>
-      </c>
+      <c r="B21" s="33" t="n"/>
+      <c r="C21" s="33" t="n"/>
+      <c r="D21" s="33" t="n"/>
       <c r="E21" s="33" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>-</t>
         </is>
       </c>
       <c r="F21" s="71">
         <f>IFERROR((VLOOKUP(E21,$AE$11:$AG$14,3,0)),"-")</f>
         <v/>
       </c>
-      <c r="G21" s="33" t="inlineStr">
-        <is>
-          <t>JN-A-0-D-N0/800x400/N/00/000</t>
-        </is>
-      </c>
-      <c r="H21" s="33" t="n">
-        <v>90261029</v>
-      </c>
-      <c r="I21" s="46" t="n">
-        <v>451.44</v>
-      </c>
-      <c r="J21" s="35" t="n">
-        <v>0</v>
-      </c>
-      <c r="K21" s="35" t="n">
-        <v>0</v>
-      </c>
+      <c r="G21" s="33" t="n"/>
+      <c r="H21" s="33" t="n"/>
+      <c r="I21" s="46" t="n"/>
+      <c r="J21" s="35" t="n"/>
+      <c r="K21" s="35" t="n"/>
       <c r="L21" s="36">
         <f>IF($H$4="-",0,IF($H$4="VAREJO",AW21,IF($H$4="ATACADO",AX21,0)))</f>
         <v/>
@@ -11284,45 +11064,23 @@
       <c r="A22" s="32" t="n">
         <v>12</v>
       </c>
-      <c r="B22" s="33" t="n">
-        <v>4</v>
-      </c>
-      <c r="C22" s="33" t="inlineStr">
-        <is>
-          <t>PÇ</t>
-        </is>
-      </c>
-      <c r="D22" s="33" t="inlineStr">
-        <is>
-          <t>010 DAMPER JN-A 0 300x200 00 000 TROX</t>
-        </is>
-      </c>
+      <c r="B22" s="33" t="n"/>
+      <c r="C22" s="33" t="n"/>
+      <c r="D22" s="33" t="n"/>
       <c r="E22" s="33" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>-</t>
         </is>
       </c>
       <c r="F22" s="71">
         <f>IFERROR((VLOOKUP(E22,$AE$11:$AG$14,3,0)),"-")</f>
         <v/>
       </c>
-      <c r="G22" s="33" t="inlineStr">
-        <is>
-          <t>JN-A-0-D-N0/300x200/N/00/000</t>
-        </is>
-      </c>
-      <c r="H22" s="33" t="n">
-        <v>90261029</v>
-      </c>
-      <c r="I22" s="46" t="n">
-        <v>195.91</v>
-      </c>
-      <c r="J22" s="35" t="n">
-        <v>0</v>
-      </c>
-      <c r="K22" s="35" t="n">
-        <v>0</v>
-      </c>
+      <c r="G22" s="33" t="n"/>
+      <c r="H22" s="33" t="n"/>
+      <c r="I22" s="46" t="n"/>
+      <c r="J22" s="35" t="n"/>
+      <c r="K22" s="35" t="n"/>
       <c r="L22" s="36">
         <f>IF($H$4="-",0,IF($H$4="VAREJO",AW22,IF($H$4="ATACADO",AX22,0)))</f>
         <v/>
@@ -11368,45 +11126,23 @@
       <c r="A23" s="32" t="n">
         <v>13</v>
       </c>
-      <c r="B23" s="33" t="n">
-        <v>1</v>
-      </c>
-      <c r="C23" s="33" t="inlineStr">
-        <is>
-          <t>PÇ</t>
-        </is>
-      </c>
-      <c r="D23" s="33" t="inlineStr">
-        <is>
-          <t>010 DAMPER RG-B 300x105 TROX</t>
-        </is>
-      </c>
+      <c r="B23" s="33" t="n"/>
+      <c r="C23" s="33" t="n"/>
+      <c r="D23" s="33" t="n"/>
       <c r="E23" s="33" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>-</t>
         </is>
       </c>
       <c r="F23" s="71">
         <f>IFERROR((VLOOKUP(E23,$AE$11:$AG$14,3,0)),"-")</f>
         <v/>
       </c>
-      <c r="G23" s="33" t="inlineStr">
-        <is>
-          <t>RG-B-300x105/D/0/00/000</t>
-        </is>
-      </c>
-      <c r="H23" s="33" t="n">
-        <v>90261029</v>
-      </c>
-      <c r="I23" s="46" t="n">
-        <v>77.29000000000001</v>
-      </c>
-      <c r="J23" s="35" t="n">
-        <v>0</v>
-      </c>
-      <c r="K23" s="35" t="n">
-        <v>0</v>
-      </c>
+      <c r="G23" s="33" t="n"/>
+      <c r="H23" s="33" t="n"/>
+      <c r="I23" s="46" t="n"/>
+      <c r="J23" s="35" t="n"/>
+      <c r="K23" s="35" t="n"/>
       <c r="L23" s="36">
         <f>IF($H$4="-",0,IF($H$4="VAREJO",AW23,IF($H$4="ATACADO",AX23,0)))</f>
         <v/>
@@ -11452,45 +11188,23 @@
       <c r="A24" s="32" t="n">
         <v>14</v>
       </c>
-      <c r="B24" s="33" t="n">
-        <v>2</v>
-      </c>
-      <c r="C24" s="33" t="inlineStr">
-        <is>
-          <t>PÇ</t>
-        </is>
-      </c>
-      <c r="D24" s="33" t="inlineStr">
-        <is>
-          <t>010 DAMPER RG-B 300x155 TROX</t>
-        </is>
-      </c>
+      <c r="B24" s="33" t="n"/>
+      <c r="C24" s="33" t="n"/>
+      <c r="D24" s="33" t="n"/>
       <c r="E24" s="33" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>-</t>
         </is>
       </c>
       <c r="F24" s="71">
         <f>IFERROR((VLOOKUP(E24,$AE$11:$AG$14,3,0)),"-")</f>
         <v/>
       </c>
-      <c r="G24" s="33" t="inlineStr">
-        <is>
-          <t>RG-B-300x155/D/0/00/000</t>
-        </is>
-      </c>
-      <c r="H24" s="33" t="n">
-        <v>90261029</v>
-      </c>
-      <c r="I24" s="46" t="n">
-        <v>88.16</v>
-      </c>
-      <c r="J24" s="35" t="n">
-        <v>0</v>
-      </c>
-      <c r="K24" s="35" t="n">
-        <v>0</v>
-      </c>
+      <c r="G24" s="33" t="n"/>
+      <c r="H24" s="33" t="n"/>
+      <c r="I24" s="46" t="n"/>
+      <c r="J24" s="35" t="n"/>
+      <c r="K24" s="35" t="n"/>
       <c r="L24" s="36">
         <f>IF($H$4="-",0,IF($H$4="VAREJO",AW24,IF($H$4="ATACADO",AX24,0)))</f>
         <v/>
@@ -11536,45 +11250,23 @@
       <c r="A25" s="32" t="n">
         <v>15</v>
       </c>
-      <c r="B25" s="33" t="n">
-        <v>6</v>
-      </c>
-      <c r="C25" s="33" t="inlineStr">
-        <is>
-          <t>PÇ</t>
-        </is>
-      </c>
-      <c r="D25" s="33" t="inlineStr">
-        <is>
-          <t>010 GRELHA AR-AG 150x145 AN0 TROX</t>
-        </is>
-      </c>
+      <c r="B25" s="33" t="n"/>
+      <c r="C25" s="33" t="n"/>
+      <c r="D25" s="33" t="n"/>
       <c r="E25" s="33" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>-</t>
         </is>
       </c>
       <c r="F25" s="71">
         <f>IFERROR((VLOOKUP(E25,$AE$11:$AG$14,3,0)),"-")</f>
         <v/>
       </c>
-      <c r="G25" s="33" t="inlineStr">
-        <is>
-          <t>AR-AG-150x145/0/0/FAN0M0</t>
-        </is>
-      </c>
-      <c r="H25" s="33" t="n">
-        <v>76169900</v>
-      </c>
-      <c r="I25" s="46" t="n">
-        <v>70.01000000000001</v>
-      </c>
-      <c r="J25" s="35" t="n">
-        <v>0</v>
-      </c>
-      <c r="K25" s="35" t="n">
-        <v>0.0325</v>
-      </c>
+      <c r="G25" s="33" t="n"/>
+      <c r="H25" s="33" t="n"/>
+      <c r="I25" s="46" t="n"/>
+      <c r="J25" s="35" t="n"/>
+      <c r="K25" s="35" t="n"/>
       <c r="L25" s="36">
         <f>IF($H$4="-",0,IF($H$4="VAREJO",AW25,IF($H$4="ATACADO",AX25,0)))</f>
         <v/>
@@ -11620,45 +11312,23 @@
       <c r="A26" s="32" t="n">
         <v>16</v>
       </c>
-      <c r="B26" s="33" t="n">
-        <v>29</v>
-      </c>
-      <c r="C26" s="33" t="inlineStr">
-        <is>
-          <t>PÇ</t>
-        </is>
-      </c>
-      <c r="D26" s="33" t="inlineStr">
-        <is>
-          <t>010 GRELHA AR-AG 250x205 AN0 TROX</t>
-        </is>
-      </c>
+      <c r="B26" s="33" t="n"/>
+      <c r="C26" s="33" t="n"/>
+      <c r="D26" s="33" t="n"/>
       <c r="E26" s="33" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>-</t>
         </is>
       </c>
       <c r="F26" s="71">
         <f>IFERROR((VLOOKUP(E26,$AE$11:$AG$14,3,0)),"-")</f>
         <v/>
       </c>
-      <c r="G26" s="33" t="inlineStr">
-        <is>
-          <t>AR-AG-250x205/0/0/FAN0M0</t>
-        </is>
-      </c>
-      <c r="H26" s="33" t="n">
-        <v>76169900</v>
-      </c>
-      <c r="I26" s="46" t="n">
-        <v>95.22</v>
-      </c>
-      <c r="J26" s="35" t="n">
-        <v>0</v>
-      </c>
-      <c r="K26" s="35" t="n">
-        <v>0.0325</v>
-      </c>
+      <c r="G26" s="33" t="n"/>
+      <c r="H26" s="33" t="n"/>
+      <c r="I26" s="46" t="n"/>
+      <c r="J26" s="35" t="n"/>
+      <c r="K26" s="35" t="n"/>
       <c r="L26" s="36">
         <f>IF($H$4="-",0,IF($H$4="VAREJO",AW26,IF($H$4="ATACADO",AX26,0)))</f>
         <v/>
@@ -11704,45 +11374,23 @@
       <c r="A27" s="32" t="n">
         <v>17</v>
       </c>
-      <c r="B27" s="33" t="n">
-        <v>1</v>
-      </c>
-      <c r="C27" s="33" t="inlineStr">
-        <is>
-          <t>PÇ</t>
-        </is>
-      </c>
-      <c r="D27" s="33" t="inlineStr">
-        <is>
-          <t>010 TOMADA DE AR VDF F711 AWK 947x797  TROX</t>
-        </is>
-      </c>
+      <c r="B27" s="33" t="n"/>
+      <c r="C27" s="33" t="n"/>
+      <c r="D27" s="33" t="n"/>
       <c r="E27" s="33" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>-</t>
         </is>
       </c>
       <c r="F27" s="71">
         <f>IFERROR((VLOOKUP(E27,$AE$11:$AG$14,3,0)),"-")</f>
         <v/>
       </c>
-      <c r="G27" s="33" t="inlineStr">
-        <is>
-          <t>VDF-F711/947x797/K/AG/F/AN0</t>
-        </is>
-      </c>
-      <c r="H27" s="33" t="n">
-        <v>76169900</v>
-      </c>
-      <c r="I27" s="46" t="n">
-        <v>625.96</v>
-      </c>
-      <c r="J27" s="35" t="n">
-        <v>0</v>
-      </c>
-      <c r="K27" s="35" t="n">
-        <v>0.0325</v>
-      </c>
+      <c r="G27" s="33" t="n"/>
+      <c r="H27" s="33" t="n"/>
+      <c r="I27" s="46" t="n"/>
+      <c r="J27" s="35" t="n"/>
+      <c r="K27" s="35" t="n"/>
       <c r="L27" s="36">
         <f>IF($H$4="-",0,IF($H$4="VAREJO",AW27,IF($H$4="ATACADO",AX27,0)))</f>
         <v/>
@@ -11788,45 +11436,23 @@
       <c r="A28" s="32" t="n">
         <v>18</v>
       </c>
-      <c r="B28" s="33" t="n">
-        <v>1</v>
-      </c>
-      <c r="C28" s="33" t="inlineStr">
-        <is>
-          <t>PÇ</t>
-        </is>
-      </c>
-      <c r="D28" s="33" t="inlineStr">
-        <is>
-          <t>010 DAMPER JN-A 0 800x400 00 000 TROX</t>
-        </is>
-      </c>
+      <c r="B28" s="33" t="n"/>
+      <c r="C28" s="33" t="n"/>
+      <c r="D28" s="33" t="n"/>
       <c r="E28" s="33" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>-</t>
         </is>
       </c>
       <c r="F28" s="71">
         <f>IFERROR((VLOOKUP(E28,$AE$11:$AG$14,3,0)),"-")</f>
         <v/>
       </c>
-      <c r="G28" s="33" t="inlineStr">
-        <is>
-          <t>JN-A-0-D-N0/800x400/N/00/000</t>
-        </is>
-      </c>
-      <c r="H28" s="33" t="n">
-        <v>90261029</v>
-      </c>
-      <c r="I28" s="46" t="n">
-        <v>451.44</v>
-      </c>
-      <c r="J28" s="35" t="n">
-        <v>0</v>
-      </c>
-      <c r="K28" s="35" t="n">
-        <v>0</v>
-      </c>
+      <c r="G28" s="33" t="n"/>
+      <c r="H28" s="33" t="n"/>
+      <c r="I28" s="46" t="n"/>
+      <c r="J28" s="35" t="n"/>
+      <c r="K28" s="35" t="n"/>
       <c r="L28" s="36">
         <f>IF($H$4="-",0,IF($H$4="VAREJO",AW28,IF($H$4="ATACADO",AX28,0)))</f>
         <v/>
@@ -11872,45 +11498,23 @@
       <c r="A29" s="32" t="n">
         <v>19</v>
       </c>
-      <c r="B29" s="33" t="n">
-        <v>1</v>
-      </c>
-      <c r="C29" s="33" t="inlineStr">
-        <is>
-          <t>PÇ</t>
-        </is>
-      </c>
-      <c r="D29" s="33" t="inlineStr">
-        <is>
-          <t>010 DAMPER JN-A 0 500x300 00 000 TROX</t>
-        </is>
-      </c>
+      <c r="B29" s="33" t="n"/>
+      <c r="C29" s="33" t="n"/>
+      <c r="D29" s="33" t="n"/>
       <c r="E29" s="33" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>-</t>
         </is>
       </c>
       <c r="F29" s="71">
         <f>IFERROR((VLOOKUP(E29,$AE$11:$AG$14,3,0)),"-")</f>
         <v/>
       </c>
-      <c r="G29" s="33" t="inlineStr">
-        <is>
-          <t>JN-A-0-D-N0/500x300/N/00/000</t>
-        </is>
-      </c>
-      <c r="H29" s="33" t="n">
-        <v>90261029</v>
-      </c>
-      <c r="I29" s="46" t="n">
-        <v>302.27</v>
-      </c>
-      <c r="J29" s="35" t="n">
-        <v>0</v>
-      </c>
-      <c r="K29" s="35" t="n">
-        <v>0</v>
-      </c>
+      <c r="G29" s="33" t="n"/>
+      <c r="H29" s="33" t="n"/>
+      <c r="I29" s="46" t="n"/>
+      <c r="J29" s="35" t="n"/>
+      <c r="K29" s="35" t="n"/>
       <c r="L29" s="36">
         <f>IF($H$4="-",0,IF($H$4="VAREJO",AW29,IF($H$4="ATACADO",AX29,0)))</f>
         <v/>
@@ -11956,45 +11560,23 @@
       <c r="A30" s="32" t="n">
         <v>20</v>
       </c>
-      <c r="B30" s="33" t="n">
-        <v>1</v>
-      </c>
-      <c r="C30" s="33" t="inlineStr">
-        <is>
-          <t>PÇ</t>
-        </is>
-      </c>
-      <c r="D30" s="33" t="inlineStr">
-        <is>
-          <t>010 DAMPER RG-B 300x155 TROX</t>
-        </is>
-      </c>
+      <c r="B30" s="33" t="n"/>
+      <c r="C30" s="33" t="n"/>
+      <c r="D30" s="33" t="n"/>
       <c r="E30" s="33" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>-</t>
         </is>
       </c>
       <c r="F30" s="71">
         <f>IFERROR((VLOOKUP(E30,$AE$11:$AG$14,3,0)),"-")</f>
         <v/>
       </c>
-      <c r="G30" s="33" t="inlineStr">
-        <is>
-          <t>RG-B-300x155/D/0/00/000</t>
-        </is>
-      </c>
-      <c r="H30" s="33" t="n">
-        <v>90261029</v>
-      </c>
-      <c r="I30" s="46" t="n">
-        <v>88.16</v>
-      </c>
-      <c r="J30" s="35" t="n">
-        <v>0</v>
-      </c>
-      <c r="K30" s="35" t="n">
-        <v>0</v>
-      </c>
+      <c r="G30" s="33" t="n"/>
+      <c r="H30" s="33" t="n"/>
+      <c r="I30" s="46" t="n"/>
+      <c r="J30" s="35" t="n"/>
+      <c r="K30" s="35" t="n"/>
       <c r="L30" s="36">
         <f>IF($H$4="-",0,IF($H$4="VAREJO",AW30,IF($H$4="ATACADO",AX30,0)))</f>
         <v/>
@@ -12040,45 +11622,23 @@
       <c r="A31" s="32" t="n">
         <v>21</v>
       </c>
-      <c r="B31" s="33" t="n">
-        <v>8</v>
-      </c>
-      <c r="C31" s="33" t="inlineStr">
-        <is>
-          <t>PÇ</t>
-        </is>
-      </c>
-      <c r="D31" s="33" t="inlineStr">
-        <is>
-          <t>010 GRELHA VAT-DG 405x400 TROX</t>
-        </is>
-      </c>
+      <c r="B31" s="33" t="n"/>
+      <c r="C31" s="33" t="n"/>
+      <c r="D31" s="33" t="n"/>
       <c r="E31" s="33" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>-</t>
         </is>
       </c>
       <c r="F31" s="71">
         <f>IFERROR((VLOOKUP(E31,$AE$11:$AG$14,3,0)),"-")</f>
         <v/>
       </c>
-      <c r="G31" s="33" t="inlineStr">
-        <is>
-          <t>VAT-0-DG405x400/00FAN0M0</t>
-        </is>
-      </c>
-      <c r="H31" s="33" t="n">
-        <v>76169900</v>
-      </c>
-      <c r="I31" s="46" t="n">
-        <v>218.19</v>
-      </c>
-      <c r="J31" s="35" t="n">
-        <v>0</v>
-      </c>
-      <c r="K31" s="35" t="n">
-        <v>0.0325</v>
-      </c>
+      <c r="G31" s="33" t="n"/>
+      <c r="H31" s="33" t="n"/>
+      <c r="I31" s="46" t="n"/>
+      <c r="J31" s="35" t="n"/>
+      <c r="K31" s="35" t="n"/>
       <c r="L31" s="36">
         <f>IF($H$4="-",0,IF($H$4="VAREJO",AW31,IF($H$4="ATACADO",AX31,0)))</f>
         <v/>
@@ -12124,45 +11684,23 @@
       <c r="A32" s="32" t="n">
         <v>22</v>
       </c>
-      <c r="B32" s="33" t="n">
-        <v>1</v>
-      </c>
-      <c r="C32" s="33" t="inlineStr">
-        <is>
-          <t>PÇ</t>
-        </is>
-      </c>
-      <c r="D32" s="33" t="inlineStr">
-        <is>
-          <t>010 GRELHA VAT-DG 245x250 TROX</t>
-        </is>
-      </c>
+      <c r="B32" s="33" t="n"/>
+      <c r="C32" s="33" t="n"/>
+      <c r="D32" s="33" t="n"/>
       <c r="E32" s="33" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>-</t>
         </is>
       </c>
       <c r="F32" s="71">
         <f>IFERROR((VLOOKUP(E32,$AE$11:$AG$14,3,0)),"-")</f>
         <v/>
       </c>
-      <c r="G32" s="33" t="inlineStr">
-        <is>
-          <t>VAT-0-DG245x250/00FAN0M0</t>
-        </is>
-      </c>
-      <c r="H32" s="33" t="n">
-        <v>76169900</v>
-      </c>
-      <c r="I32" s="46" t="n">
-        <v>123.44</v>
-      </c>
-      <c r="J32" s="35" t="n">
-        <v>0</v>
-      </c>
-      <c r="K32" s="35" t="n">
-        <v>0.0325</v>
-      </c>
+      <c r="G32" s="33" t="n"/>
+      <c r="H32" s="33" t="n"/>
+      <c r="I32" s="46" t="n"/>
+      <c r="J32" s="35" t="n"/>
+      <c r="K32" s="35" t="n"/>
       <c r="L32" s="36">
         <f>IF($H$4="-",0,IF($H$4="VAREJO",AW32,IF($H$4="ATACADO",AX32,0)))</f>
         <v/>
@@ -12208,45 +11746,23 @@
       <c r="A33" s="32" t="n">
         <v>23</v>
       </c>
-      <c r="B33" s="33" t="n">
-        <v>1</v>
-      </c>
-      <c r="C33" s="33" t="inlineStr">
-        <is>
-          <t>PÇ</t>
-        </is>
-      </c>
-      <c r="D33" s="33" t="inlineStr">
-        <is>
-          <t>010 DAMPER RG-B 250x155 TROX</t>
-        </is>
-      </c>
+      <c r="B33" s="33" t="n"/>
+      <c r="C33" s="33" t="n"/>
+      <c r="D33" s="33" t="n"/>
       <c r="E33" s="33" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>-</t>
         </is>
       </c>
       <c r="F33" s="71">
         <f>IFERROR((VLOOKUP(E33,$AE$11:$AG$14,3,0)),"-")</f>
         <v/>
       </c>
-      <c r="G33" s="33" t="inlineStr">
-        <is>
-          <t>RG-B-250x155/D/0/00/000</t>
-        </is>
-      </c>
-      <c r="H33" s="33" t="n">
-        <v>90261029</v>
-      </c>
-      <c r="I33" s="46" t="n">
-        <v>82.65000000000001</v>
-      </c>
-      <c r="J33" s="35" t="n">
-        <v>0</v>
-      </c>
-      <c r="K33" s="35" t="n">
-        <v>0</v>
-      </c>
+      <c r="G33" s="33" t="n"/>
+      <c r="H33" s="33" t="n"/>
+      <c r="I33" s="46" t="n"/>
+      <c r="J33" s="35" t="n"/>
+      <c r="K33" s="35" t="n"/>
       <c r="L33" s="36">
         <f>IF($H$4="-",0,IF($H$4="VAREJO",AW33,IF($H$4="ATACADO",AX33,0)))</f>
         <v/>

</xml_diff>